<commit_message>
updated spreadsheet coefficients to compute grams per week
</commit_message>
<xml_diff>
--- a/spreadsheets/ewac-spreadsheet.xlsx
+++ b/spreadsheets/ewac-spreadsheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
   <si>
     <t xml:space="preserve">person_id</t>
   </si>
@@ -35,7 +35,10 @@
     <t xml:space="preserve">audit3</t>
   </si>
   <si>
-    <t xml:space="preserve">EWAC</t>
+    <t xml:space="preserve">EWAC_grams_week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EWAC_UK_units_week</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -144,10 +147,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0"/>
+    <numFmt numFmtId="169" formatCode="0.00000000"/>
+    <numFmt numFmtId="170" formatCode="0.000000000"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -218,7 +226,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,11 +235,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,16 +280,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -280,207 +309,286 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="n">
         <f aca="false">((INDEX(Extended_AUDIT_Look_Up!$D$4:$D$9,MATCH(B2,Extended_AUDIT_Look_Up!$C$4:$C$9,0))*INDEX(Extended_AUDIT_Look_Up!$D$14:$D$20,MATCH(C2,Extended_AUDIT_Look_Up!$C$14:$C$20,0)))+INDEX(Extended_AUDIT_Look_Up!$D$25:$D$29,MATCH(D2,Extended_AUDIT_Look_Up!$C$25:$C$29,0)))</f>
-        <v>1.336586</v>
-      </c>
+        <v>10.6794111984</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <f aca="false">E2/8</f>
+        <v>1.3349263998</v>
+      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="n">
         <f aca="false">((INDEX(Extended_AUDIT_Look_Up!$D$4:$D$9,MATCH(B3,Extended_AUDIT_Look_Up!$C$4:$C$9,0))*INDEX(Extended_AUDIT_Look_Up!$D$14:$D$20,MATCH(C3,Extended_AUDIT_Look_Up!$C$14:$C$20,0)))+INDEX(Extended_AUDIT_Look_Up!$D$25:$D$29,MATCH(D3,Extended_AUDIT_Look_Up!$C$25:$C$29,0)))</f>
-        <v>5.784108</v>
-      </c>
+        <v>46.2766288048</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <f aca="false">E3/8</f>
+        <v>5.7845786006</v>
+      </c>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="n">
         <f aca="false">((INDEX(Extended_AUDIT_Look_Up!$D$4:$D$9,MATCH(B4,Extended_AUDIT_Look_Up!$C$4:$C$9,0))*INDEX(Extended_AUDIT_Look_Up!$D$14:$D$20,MATCH(C4,Extended_AUDIT_Look_Up!$C$14:$C$20,0)))+INDEX(Extended_AUDIT_Look_Up!$D$25:$D$29,MATCH(D4,Extended_AUDIT_Look_Up!$C$25:$C$29,0)))</f>
-        <v>14.812988</v>
-      </c>
+        <v>118.5000785328</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <f aca="false">E4/8</f>
+        <v>14.8125098166</v>
+      </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="n">
         <f aca="false">((INDEX(Extended_AUDIT_Look_Up!$D$4:$D$9,MATCH(B5,Extended_AUDIT_Look_Up!$C$4:$C$9,0))*INDEX(Extended_AUDIT_Look_Up!$D$14:$D$20,MATCH(C5,Extended_AUDIT_Look_Up!$C$14:$C$20,0)))+INDEX(Extended_AUDIT_Look_Up!$D$25:$D$29,MATCH(D5,Extended_AUDIT_Look_Up!$C$25:$C$29,0)))</f>
-        <v>13.08796</v>
-      </c>
+        <v>104.7057829232</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <f aca="false">E5/8</f>
+        <v>13.0882228654</v>
+      </c>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="n">
         <f aca="false">((INDEX(Extended_AUDIT_Look_Up!$D$4:$D$9,MATCH(B6,Extended_AUDIT_Look_Up!$C$4:$C$9,0))*INDEX(Extended_AUDIT_Look_Up!$D$14:$D$20,MATCH(C6,Extended_AUDIT_Look_Up!$C$14:$C$20,0)))+INDEX(Extended_AUDIT_Look_Up!$D$25:$D$29,MATCH(D6,Extended_AUDIT_Look_Up!$C$25:$C$29,0)))</f>
-        <v>8.59515</v>
-      </c>
+        <v>68.7701833408</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <f aca="false">E6/8</f>
+        <v>8.5962729176</v>
+      </c>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="n">
         <f aca="false">((INDEX(Extended_AUDIT_Look_Up!$D$4:$D$9,MATCH(B7,Extended_AUDIT_Look_Up!$C$4:$C$9,0))*INDEX(Extended_AUDIT_Look_Up!$D$14:$D$20,MATCH(C7,Extended_AUDIT_Look_Up!$C$14:$C$20,0)))+INDEX(Extended_AUDIT_Look_Up!$D$25:$D$29,MATCH(D7,Extended_AUDIT_Look_Up!$C$25:$C$29,0)))</f>
-        <v>30.80356</v>
-      </c>
+        <v>246.4284816752</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <f aca="false">E7/8</f>
+        <v>30.8035602094</v>
+      </c>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1" t="n">
         <f aca="false">((INDEX(Extended_AUDIT_Look_Up!$D$4:$D$9,MATCH(B8,Extended_AUDIT_Look_Up!$C$4:$C$9,0))*INDEX(Extended_AUDIT_Look_Up!$D$14:$D$20,MATCH(C8,Extended_AUDIT_Look_Up!$C$14:$C$20,0)))+INDEX(Extended_AUDIT_Look_Up!$D$25:$D$29,MATCH(D8,Extended_AUDIT_Look_Up!$C$25:$C$29,0)))</f>
-        <v>7.549988</v>
-      </c>
+        <v>60.4032275328</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <f aca="false">E8/8</f>
+        <v>7.5504034416</v>
+      </c>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="n">
         <f aca="false">((INDEX(Extended_AUDIT_Look_Up!$D$4:$D$9,MATCH(B9,Extended_AUDIT_Look_Up!$C$4:$C$9,0))*INDEX(Extended_AUDIT_Look_Up!$D$14:$D$20,MATCH(C9,Extended_AUDIT_Look_Up!$C$14:$C$20,0)))+INDEX(Extended_AUDIT_Look_Up!$D$25:$D$29,MATCH(D9,Extended_AUDIT_Look_Up!$C$25:$C$29,0)))</f>
-        <v>0.985226</v>
-      </c>
+        <v>7.8759900144</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <f aca="false">E9/8</f>
+        <v>0.9844987518</v>
+      </c>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" s="1" t="n">
         <f aca="false">((INDEX(Extended_AUDIT_Look_Up!$D$4:$D$9,MATCH(B10,Extended_AUDIT_Look_Up!$C$4:$C$9,0))*INDEX(Extended_AUDIT_Look_Up!$D$14:$D$20,MATCH(C10,Extended_AUDIT_Look_Up!$C$14:$C$20,0)))+INDEX(Extended_AUDIT_Look_Up!$D$25:$D$29,MATCH(D10,Extended_AUDIT_Look_Up!$C$25:$C$29,0)))</f>
-        <v>14.97915</v>
-      </c>
+        <v>119.8464580288</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <f aca="false">E10/8</f>
+        <v>14.9808072536</v>
+      </c>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="n">
         <f aca="false">((INDEX(Extended_AUDIT_Look_Up!$D$4:$D$9,MATCH(B11,Extended_AUDIT_Look_Up!$C$4:$C$9,0))*INDEX(Extended_AUDIT_Look_Up!$D$14:$D$20,MATCH(C11,Extended_AUDIT_Look_Up!$C$14:$C$20,0)))+INDEX(Extended_AUDIT_Look_Up!$D$25:$D$29,MATCH(D11,Extended_AUDIT_Look_Up!$C$25:$C$29,0)))</f>
-        <v>62.52756</v>
-      </c>
+        <v>500.2210536752</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <f aca="false">E11/8</f>
+        <v>62.5276317094</v>
+      </c>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="1"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="1"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2"/>
+      <c r="B17" s="4"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2"/>
+      <c r="B18" s="4"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F26" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -498,31 +606,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E29"/>
+  <dimension ref="A2:E30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,12 +641,12 @@
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -548,12 +656,12 @@
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>0.183</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>0.1825144</v>
+      </c>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -563,12 +671,12 @@
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>0.562</v>
-      </c>
-      <c r="E6" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>0.5622265</v>
+      </c>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -578,12 +686,12 @@
         <v>3</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>1.614</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>1.6139923</v>
+      </c>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -593,12 +701,12 @@
         <v>4</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>3.325</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>3.3252783</v>
+      </c>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -608,30 +716,30 @@
         <v>4</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>5.18</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>5.1799232</v>
+      </c>
+      <c r="E9" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,10 +750,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>2.422</v>
+        <v>12</v>
+      </c>
+      <c r="D14" s="8" t="n">
+        <v>19.376</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,10 +764,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>4.342</v>
+        <v>8</v>
+      </c>
+      <c r="D15" s="8" t="n">
+        <v>34.736</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,10 +778,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>5.842</v>
+        <v>21</v>
+      </c>
+      <c r="D16" s="8" t="n">
+        <v>46.736</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -684,10 +792,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>6.891</v>
+        <v>34</v>
+      </c>
+      <c r="D17" s="8" t="n">
+        <v>55.128</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -698,10 +806,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>9.67</v>
+        <v>35</v>
+      </c>
+      <c r="D18" s="8" t="n">
+        <v>77.36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,10 +820,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>9.725</v>
+        <v>36</v>
+      </c>
+      <c r="D19" s="8" t="n">
+        <v>77.8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -726,29 +834,29 @@
         <v>4</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>17.832</v>
+        <v>37</v>
+      </c>
+      <c r="D20" s="8" t="n">
+        <v>142.656</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,12 +867,12 @@
         <v>0</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>0.542</v>
-      </c>
-      <c r="E25" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="D25" s="8" t="n">
+        <v>4.339591</v>
+      </c>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -774,12 +882,12 @@
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="0" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="E26" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="D26" s="8" t="n">
+        <v>15.003914</v>
+      </c>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -789,12 +897,12 @@
         <v>2</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="0" t="n">
-        <v>3.656</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="D27" s="8" t="n">
+        <v>29.249415</v>
+      </c>
+      <c r="E27" s="6"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -804,12 +912,12 @@
         <v>3</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>7.805</v>
-      </c>
-      <c r="E28" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="D28" s="8" t="n">
+        <v>62.436442</v>
+      </c>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -819,12 +927,15 @@
         <v>4</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D29" s="0" t="n">
-        <v>32.266</v>
-      </c>
-      <c r="E29" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="D29" s="8" t="n">
+        <v>258.132163</v>
+      </c>
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>